<commit_message>
add network config flash and tested
</commit_message>
<xml_diff>
--- a/wifi_bt_xbr/DOC/flash分配.xlsx
+++ b/wifi_bt_xbr/DOC/flash分配.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="51">
   <si>
     <t>全局变量</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -86,10 +86,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>蓝牙重新连接次数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>感应延时</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -194,11 +190,36 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0x0C</t>
+    <t>USER_PARAMETER_START_SECTOR_ADDRESS0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>USER_PARAMETER_START_SECTOR_ADDRESS1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wifi_join_cnt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>重新连接次数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>首次连接标志</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -230,7 +251,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -253,39 +274,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -295,10 +290,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -600,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -613,7 +605,8 @@
     <col min="3" max="3" width="10.9296875" style="2" customWidth="1"/>
     <col min="4" max="4" width="21.73046875" style="2" customWidth="1"/>
     <col min="5" max="5" width="21" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="9.06640625" style="2"/>
+    <col min="6" max="6" width="42.06640625" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.06640625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -630,27 +623,28 @@
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>33</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>45</v>
+        <v>33</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -667,7 +661,10 @@
         <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -681,10 +678,13 @@
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -701,7 +701,10 @@
         <v>14</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -715,9 +718,12 @@
         <v>6</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="4"/>
+        <v>19</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="1" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1">
@@ -733,7 +739,10 @@
         <v>16</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -750,7 +759,10 @@
         <v>15</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -758,16 +770,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -775,16 +790,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -792,16 +810,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -809,15 +830,18 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>43</v>
       </c>
     </row>
@@ -832,9 +856,32 @@
         <v>6</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>